<commit_message>
estado del arte completado documento final
</commit_message>
<xml_diff>
--- a/seleccion Biblio Estado Arte 2.0.xlsx
+++ b/seleccion Biblio Estado Arte 2.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="130">
   <si>
     <t>Titulo</t>
   </si>
@@ -264,6 +264,156 @@
   </si>
   <si>
     <t>Ok</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Internet of Things (IoT) adoption barriers of smart cities’ waste management: An Indian context</t>
+  </si>
+  <si>
+    <t>Manu Sharma,Sudhanshu Joshi, Devika Kannan, Kannan Govindan, Rohit Singh, H.C.Purohita</t>
+  </si>
+  <si>
+    <t>10.1016/j.jclepro.2020.122047</t>
+  </si>
+  <si>
+    <t>marco estructural de IoT que usa toma de decisiones multi criterio para y superacion de barreras en la implementacion de sistemas de administracion de basuras en cuidades inteligentes.</t>
+  </si>
+  <si>
+    <t>Cyber-physical System Enabled in Sustainable Waste Management 4.0: A Smart Waste Collection System for Indonesian Semi-Urban Cities</t>
+  </si>
+  <si>
+    <t>Yun Arifatul Fatimah, Andi Widianto, Muhtar Hanafi</t>
+  </si>
+  <si>
+    <t>10.1016/j.promfg.2020.02.169</t>
+  </si>
+  <si>
+    <t>el uso de sistema cyber fisicos CPS, es relevante en la mejora de prosesos como la recoleccion de residous, el objetivo del estudio es integrar los componenetes del un sistema para la administraciuon de residuo en indonesia</t>
+  </si>
+  <si>
+    <t>Enhanced Route Selection (ERS) algorithm for IoT enabled smart waste management system</t>
+  </si>
+  <si>
+    <t>Nidhy R. Manish Kumar, Renjith V. Ravi, Deepak V.</t>
+  </si>
+  <si>
+    <t>10.1016/j.eti.2020.101116</t>
+  </si>
+  <si>
+    <t>la optimizacion del proceso de recoleccion de residuos  tiene un rol importante en las cuidades inteligentes, el retrazo en la trasmicion de datos es uno de los desafios mas importantes en WSN, para superar este conflicto se propone un algoritmo eficiente para seleccion de rutas, la arquitectura propuesta es simulada en una herramienta...</t>
+  </si>
+  <si>
+    <t>Theoretical modelling and fabrication of smart waste management system for clean environment using WSN and IOT</t>
+  </si>
+  <si>
+    <t>S.Murugesan, S.Ramalingam, P.Kanimozhi</t>
+  </si>
+  <si>
+    <t>10.1016/j.matpr.2020.09.190</t>
+  </si>
+  <si>
+    <t>un sistema para determinar cuando una caneca esta proxima a llenarse y comuncar este hecho a los especialistas para que puedan limpiar rapidamente esto intentar reducir el esfuerzo humano y manejar la recoleccion de forma automatizada creando ciudadesmas inteligentes.</t>
+  </si>
+  <si>
+    <t>The interplay of circular economy with industry 4.0 enabled smart city drivers of healthcare waste disposal</t>
+  </si>
+  <si>
+    <t>Ankur Chauhan, Suresh Kumar Jakhar, Chetna Chauhan</t>
+  </si>
+  <si>
+    <t>10.1016/j.jclepro.2020.123854</t>
+  </si>
+  <si>
+    <t>sistema de eliminacion inteligente de residuos biologicos generados en hospitales para reducir los niveles de contagio por manipulacion incorrecta de desechos, como modelo relacional de la industria 4.0 aplicada a la economia circular para instalaciones de salud</t>
+  </si>
+  <si>
+    <t>Industry 4.0 based sustainable circular economy approach for smart waste management system to achieve sustainable development goals: A case study of Indonesia</t>
+  </si>
+  <si>
+    <t>Yun Arifatul Fatimah, Kannan Govindan ,Rochiyati Murniningsih, Agus Setiawan</t>
+  </si>
+  <si>
+    <t>10.1016/j.jclepro.2020.122263#</t>
+  </si>
+  <si>
+    <t>el objetivo del articulo es investigar los conflictos y oportunidades para el desarrollo de un sistema inteligente de recoleccion de residuos en indonesia y determinar una estrategia para disminuir  los problemas de recoleccion de residuos.</t>
+  </si>
+  <si>
+    <t>A stochastic optimization framework for planning of waste collection and value recovery operations in smart and sustainable cities</t>
+  </si>
+  <si>
+    <t>ParthJ atinkumar Shah, Theodoros Anagnostopoulos, Arkady Zaslavsky, Sara Behdad</t>
+  </si>
+  <si>
+    <t>se resalta la inportancia de recuperar el valor de las canecas de basura, un modelo de optimizacion estocastico basado en programacion por restriccion y oportunidad se desarrolla para planear las operaciones de recoleccion.</t>
+  </si>
+  <si>
+    <t>Holistic Big Data Integrated Artificial Intelligent Modeling to Improve Privacy and Security in Data Management of Smart Cities</t>
+  </si>
+  <si>
+    <t>Jie Chen, Dr. L Ramanathan, Dr. Mamoun Alazab</t>
+  </si>
+  <si>
+    <t>10.1016/j.micpro.2020.103722</t>
+  </si>
+  <si>
+    <t>Solid waste collection/transport optimization and vegetation land cover estimation using Geographic Information System (GIS): A case study of a proposed smart-city</t>
+  </si>
+  <si>
+    <t>Jaydeep Lella, Venkata Ravibabu Mandla, Xuan Zhu</t>
+  </si>
+  <si>
+    <t>10.1016/j.scs.2017.08.023</t>
+  </si>
+  <si>
+    <t>Electronic waste collection systems using Internet of Things (IoT): Household electronic waste management in Malaysia</t>
+  </si>
+  <si>
+    <t>Kai DeanKang, Harnyi Kang, I.M.S.K.Ilankoon, Chun Yong Chong</t>
+  </si>
+  <si>
+    <t>10.1016/j.jclepro.2019.119801</t>
+  </si>
+  <si>
+    <t>GIS and remote sensin aproaches help to manage solid waste from generation to dumping stage this study uses the smart city of Vellore in india as case study, and present methods of solid waste managemente in collection and trasportation of waste using Gis tecniques in network analysis, the optimal waste collection and transportation routes show a 59,12% reduction in travel distance.</t>
+  </si>
+  <si>
+    <t>aquí se discute una modelamiento holistico  de Big Data integrado con inteligencia artificial, para mejorar los aspectos de privacidad y seguridad en las interfaces de administracion de las cuidades inteligentes, se incorporo un algorithmo para incorporar seguridad en la confidencialidad de la informacion de la red ademas un analisis de Volumenes de datos mejora la escalabilidad y accesibilidad de la informacion teniendo en cuenta la ubicacion de almacenamiento</t>
+  </si>
+  <si>
+    <t>este articulo discute  la aplicación de recolleccion inteligente de residuos electronicos para lo cual se diseño una caja con sensores para registrar datos del material desechado, un servicio de backend se encarga de notificar al recolector para recoger el residuo electronico cuando este supera el nivel de llenado predeterminado por ejemplo el 80%.</t>
+  </si>
+  <si>
+    <t>Waste Management System Using IoT-Based Machine Learning in University</t>
+  </si>
+  <si>
+    <t>Anh Khoa T,Phuc CLam P et al</t>
+  </si>
+  <si>
+    <t>10.1155/2020/6138637</t>
+  </si>
+  <si>
+    <t>Optimization of Organic Waste Collection for Generation of Bio Gas using IoT Techniques</t>
+  </si>
+  <si>
+    <t>Manglorkar S,Sharma A,Verma D,Rane S</t>
+  </si>
+  <si>
+    <t>10.1088/1757-899X/594/1/012026</t>
+  </si>
+  <si>
+    <t>Smart waste management using Internet of Things: A survey</t>
+  </si>
+  <si>
+    <t>Fallavi K, Ravi Kumar V, Chaithra B</t>
+  </si>
+  <si>
+    <t>10.1109/I-SMAC.2017.8058247</t>
+  </si>
+  <si>
+    <t>10.1016/j.wasman.2018.05.019</t>
   </si>
 </sst>
 </file>
@@ -287,7 +437,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +456,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -319,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -328,6 +484,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -610,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,6 +818,9 @@
       <c r="E2" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -855,6 +1018,9 @@
       <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="F12" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -912,6 +1078,9 @@
       <c r="E15" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="F15" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -929,6 +1098,9 @@
       <c r="E16" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="F16" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -966,6 +1138,9 @@
       <c r="E18" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="F18" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -983,107 +1158,263 @@
       <c r="E19" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="F19" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2020</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1130,12 +1461,21 @@
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D17" r:id="rId1" display="https://doi.org/10.1177%2F0734242X18807001"/>
     <hyperlink ref="D19" r:id="rId2" display="https://doi.org/10.1016/j.ejor.2009.01.021"/>
+    <hyperlink ref="D23" r:id="rId3" tooltip="Persistent link using digital object identifier" display="https://doi-org.ezproxy.unal.edu.co/10.1016/j.promfg.2020.02.169"/>
+    <hyperlink ref="D33" r:id="rId4" display="https://dx.doi.org/10.1109/I-SMAC.2017.8058247"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
primera version del documento completa
</commit_message>
<xml_diff>
--- a/seleccion Biblio Estado Arte 2.0.xlsx
+++ b/seleccion Biblio Estado Arte 2.0.xlsx
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>